<commit_message>
added a total adjustment and renamed some files
</commit_message>
<xml_diff>
--- a/etc/calculations.xlsx
+++ b/etc/calculations.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>b1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -78,6 +78,30 @@
   </si>
   <si>
     <t>avg velocity excluding b2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>For B2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>center of mass adjustment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>velocity-adjustment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>avoidance-adjustment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>total</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>factor</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -201,23 +225,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="354785368"/>
-        <c:axId val="130166200"/>
+        <c:axId val="347874920"/>
+        <c:axId val="347916472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="354785368"/>
+        <c:axId val="347874920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130166200"/>
+        <c:crossAx val="347916472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="130166200"/>
+        <c:axId val="347916472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -225,7 +249,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="354785368"/>
+        <c:crossAx val="347874920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -600,10 +624,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -639,8 +663,8 @@
         <v>2</v>
       </c>
       <c r="F2">
-        <f ca="1">RANDBETWEEN(0, 5)</f>
-        <v>4</v>
+        <f t="shared" ref="F2:F8" ca="1" si="0">RANDBETWEEN(0, 5)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -660,8 +684,8 @@
         <v>5</v>
       </c>
       <c r="F3">
-        <f ca="1">RANDBETWEEN(0, 5)</f>
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -681,7 +705,7 @@
         <v>4</v>
       </c>
       <c r="F4">
-        <f ca="1">RANDBETWEEN(0, 5)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -702,14 +726,14 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <f ca="1">RANDBETWEEN(0, 5)</f>
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="F6">
-        <f ca="1">RANDBETWEEN(0, 5)</f>
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -717,8 +741,8 @@
         <v>14</v>
       </c>
       <c r="F7">
-        <f ca="1">RANDBETWEEN(0, 5)</f>
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -734,8 +758,8 @@
         <v>2</v>
       </c>
       <c r="F8">
-        <f ca="1">RANDBETWEEN(0, 5)</f>
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -796,7 +820,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -809,12 +833,12 @@
         <v>-2.5</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:4">
       <c r="B22">
         <f>(B2+B4+B5)/3</f>
         <v>-0.83333333333333337</v>
@@ -822,6 +846,71 @@
       <c r="C22">
         <f>(C2+C4+C5)/3</f>
         <v>3.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28">
+        <f>B22/B23</f>
+        <v>-8.3333333333333332E-3</v>
+      </c>
+      <c r="D28">
+        <f>C22/B23</f>
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29">
+        <f>D8</f>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="D29">
+        <f>E8</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30">
+        <f>B17</f>
+        <v>1.5</v>
+      </c>
+      <c r="D30">
+        <f>C17</f>
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32">
+        <f>SUM(C28:C30)</f>
+        <v>4.8250000000000002</v>
+      </c>
+      <c r="D32">
+        <f>SUM(D28:D30)</f>
+        <v>-0.46499999999999986</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed the total computation
</commit_message>
<xml_diff>
--- a/etc/calculations.xlsx
+++ b/etc/calculations.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>b1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -102,6 +102,14 @@
   </si>
   <si>
     <t>factor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bounds-adjustment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>For B5: -6 6</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -624,10 +632,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -664,7 +672,7 @@
       </c>
       <c r="F2">
         <f t="shared" ref="F2:F8" ca="1" si="0">RANDBETWEEN(0, 5)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -706,7 +714,7 @@
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -727,13 +735,13 @@
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -742,7 +750,7 @@
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -913,7 +921,73 @@
         <v>-0.46499999999999986</v>
       </c>
     </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37">
+        <f>0.01*SUM(B2:B5)/4</f>
+        <v>-1.25E-3</v>
+      </c>
+      <c r="D37">
+        <f>0.01*SUM(C2:C5)/4</f>
+        <v>2.8750000000000001E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38">
+        <f>SUM(D2:D5)/4</f>
+        <v>3.25</v>
+      </c>
+      <c r="D38">
+        <f>SUM(E2:E5)/4</f>
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39">
+        <f>-6.5-B5</f>
+        <v>-1.5</v>
+      </c>
+      <c r="D39">
+        <f>6-C5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="C41">
+        <f>SUM(C37:C40)</f>
+        <v>2.7487499999999998</v>
+      </c>
+      <c r="D41">
+        <f>SUM(D37:D40)</f>
+        <v>2.7787500000000001</v>
+      </c>
+    </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Added test for moving boid one step
</commit_message>
<xml_diff>
--- a/etc/calculations.xlsx
+++ b/etc/calculations.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>b1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -110,6 +110,18 @@
   </si>
   <si>
     <t>For B5: -6 6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>self-velocity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">New Boid </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>self-velocity</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -233,23 +245,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="347874920"/>
-        <c:axId val="347916472"/>
+        <c:axId val="417170072"/>
+        <c:axId val="417163544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="347874920"/>
+        <c:axId val="417170072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="347916472"/>
+        <c:crossAx val="417163544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="347916472"/>
+        <c:axId val="417163544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -257,7 +269,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="347874920"/>
+        <c:crossAx val="417170072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -288,7 +300,7 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>584200</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -632,10 +644,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -672,7 +684,7 @@
       </c>
       <c r="F2">
         <f t="shared" ref="F2:F8" ca="1" si="0">RANDBETWEEN(0, 5)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -693,7 +705,7 @@
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -714,7 +726,7 @@
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -735,13 +747,13 @@
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -750,7 +762,7 @@
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -767,7 +779,7 @@
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -908,17 +920,28 @@
         <v>-2.5</v>
       </c>
     </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31">
+        <v>5</v>
+      </c>
+    </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>19</v>
       </c>
       <c r="C32">
-        <f>SUM(C28:C30)</f>
-        <v>4.8250000000000002</v>
+        <f>SUM(C28:C31)</f>
+        <v>7.8250000000000002</v>
       </c>
       <c r="D32">
-        <f>SUM(D28:D30)</f>
-        <v>-0.46499999999999986</v>
+        <f>SUM(D28:D31)</f>
+        <v>4.5350000000000001</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -977,17 +1000,40 @@
       </c>
     </row>
     <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>23</v>
+      </c>
       <c r="C41">
-        <f>SUM(C37:C40)</f>
-        <v>2.7487499999999998</v>
+        <v>-1</v>
       </c>
       <c r="D41">
-        <f>SUM(D37:D40)</f>
-        <v>2.7787500000000001</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="C42">
+        <f>SUM(C37:C41)</f>
+        <v>1.7487499999999998</v>
+      </c>
+      <c r="D42">
+        <f>SUM(D37:D41)</f>
+        <v>4.7787500000000005</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>24</v>
+      </c>
+      <c r="C45">
+        <f>-6+C42</f>
+        <v>-4.2512500000000006</v>
+      </c>
+      <c r="D45">
+        <f>6+D42</f>
+        <v>10.77875</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Tested binding override of weights on adjustments
</commit_message>
<xml_diff>
--- a/etc/calculations.xlsx
+++ b/etc/calculations.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>b1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -122,6 +122,26 @@
   </si>
   <si>
     <t>For B5: -6.5 6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>weight</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>weighted x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>weighted y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>weight</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>weighted</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -245,23 +265,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="417170072"/>
-        <c:axId val="417163544"/>
+        <c:axId val="480119320"/>
+        <c:axId val="480022744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="417170072"/>
+        <c:axId val="480119320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="417163544"/>
+        <c:crossAx val="480022744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="417163544"/>
+        <c:axId val="480022744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -269,7 +289,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="417170072"/>
+        <c:crossAx val="480119320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -644,10 +664,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -684,7 +704,7 @@
       </c>
       <c r="F2">
         <f t="shared" ref="F2:F8" ca="1" si="0">RANDBETWEEN(0, 5)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -705,7 +725,7 @@
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -726,7 +746,7 @@
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -753,7 +773,7 @@
     <row r="6" spans="1:6">
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -762,7 +782,7 @@
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -779,7 +799,7 @@
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -840,7 +860,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -853,12 +873,12 @@
         <v>-2.5</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:7">
       <c r="B22">
         <f>(B2+B4+B5)/3</f>
         <v>-0.83333333333333337</v>
@@ -868,7 +888,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -876,12 +896,21 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27" t="s">
+        <v>26</v>
+      </c>
+      <c r="F27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -893,8 +922,19 @@
         <f>C22/B23</f>
         <v>3.5000000000000003E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <f>C28*E28</f>
+        <v>-8.3333333333333332E-3</v>
+      </c>
+      <c r="G28">
+        <f>E28*D28</f>
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -906,8 +946,19 @@
         <f>E8</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <f t="shared" ref="F29:F31" si="1">C29*E29</f>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="G29">
+        <f t="shared" ref="G29:G31" si="2">E29*D29</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -919,8 +970,19 @@
         <f>C17</f>
         <v>-2.5</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="2"/>
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>24</v>
       </c>
@@ -930,8 +992,19 @@
       <c r="D31">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>19</v>
       </c>
@@ -943,13 +1016,27 @@
         <f>SUM(D28:D31)</f>
         <v>4.5350000000000001</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="F32">
+        <f>SUM(F28:F31)</f>
+        <v>7.8250000000000002</v>
+      </c>
+      <c r="G32">
+        <f>SUM(G28:G31)</f>
+        <v>4.5350000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="E36" t="s">
+        <v>29</v>
+      </c>
+      <c r="F36" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>16</v>
       </c>
@@ -961,8 +1048,19 @@
         <f>0.01*SUM(C2:C5)/4</f>
         <v>2.8750000000000001E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <f>C37*E37</f>
+        <v>-1.25E-3</v>
+      </c>
+      <c r="G37">
+        <f>D37*E37</f>
+        <v>2.8750000000000001E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>17</v>
       </c>
@@ -974,8 +1072,19 @@
         <f>SUM(E2:E5)/4</f>
         <v>2.75</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <f t="shared" ref="F38:F41" si="3">C38*E38</f>
+        <v>3.25</v>
+      </c>
+      <c r="G38">
+        <f t="shared" ref="G38:G41" si="4">D38*E38</f>
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
         <v>18</v>
       </c>
@@ -987,8 +1096,19 @@
         <f>6-C5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="3"/>
+        <v>-1.5</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
         <v>21</v>
       </c>
@@ -998,8 +1118,19 @@
       <c r="D40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="E40">
+        <v>0.1</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
         <v>22</v>
       </c>
@@ -1009,8 +1140,19 @@
       <c r="D41">
         <v>2</v>
       </c>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="C42">
         <f>SUM(C37:C41)</f>
         <v>1.7487499999999998</v>
@@ -1019,8 +1161,16 @@
         <f>SUM(D37:D41)</f>
         <v>4.7787500000000005</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
+      <c r="F42">
+        <f>SUM(F37:F41)</f>
+        <v>0.84874999999999989</v>
+      </c>
+      <c r="G42">
+        <f>SUM(G37:G41)</f>
+        <v>4.7787500000000005</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Fixed the center of mass adjustment
</commit_message>
<xml_diff>
--- a/etc/calculations.xlsx
+++ b/etc/calculations.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="24720" windowHeight="17340" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="21520" windowHeight="15400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="130404" concurrentCalc="0"/>
+  <calcPr calcId="130405" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -265,23 +265,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="480119320"/>
-        <c:axId val="480022744"/>
+        <c:axId val="494715496"/>
+        <c:axId val="494711480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="480119320"/>
+        <c:axId val="494715496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="480022744"/>
+        <c:crossAx val="494711480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="480022744"/>
+        <c:axId val="494711480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -289,7 +289,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="480119320"/>
+        <c:crossAx val="494715496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -667,7 +667,7 @@
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -704,7 +704,7 @@
       </c>
       <c r="F2">
         <f t="shared" ref="F2:F8" ca="1" si="0">RANDBETWEEN(0, 5)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -725,7 +725,7 @@
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -746,7 +746,7 @@
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -773,7 +773,7 @@
     <row r="6" spans="1:6">
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -782,7 +782,7 @@
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -880,12 +880,12 @@
     </row>
     <row r="22" spans="1:7">
       <c r="B22">
-        <f>(B2+B4+B5)/3</f>
-        <v>-0.83333333333333337</v>
+        <f>(B2+B4+B5)/3-B3</f>
+        <v>-2.8333333333333335</v>
       </c>
       <c r="C22">
-        <f>(C2+C4+C5)/3</f>
-        <v>3.5</v>
+        <f>(C2+C4+C5)/3-C3</f>
+        <v>2.5</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -916,22 +916,22 @@
       </c>
       <c r="C28">
         <f>B22/B23</f>
-        <v>-8.3333333333333332E-3</v>
+        <v>-2.8333333333333335E-2</v>
       </c>
       <c r="D28">
         <f>C22/B23</f>
-        <v>3.5000000000000003E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="E28">
         <v>1</v>
       </c>
       <c r="F28">
         <f>C28*E28</f>
-        <v>-8.3333333333333332E-3</v>
+        <v>-2.8333333333333335E-2</v>
       </c>
       <c r="G28">
         <f>E28*D28</f>
-        <v>3.5000000000000003E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -971,15 +971,15 @@
         <v>-2.5</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="F30">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>0.15000000000000002</v>
       </c>
       <c r="G30">
         <f t="shared" si="2"/>
-        <v>-2.5</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1010,19 +1010,19 @@
       </c>
       <c r="C32">
         <f>SUM(C28:C31)</f>
-        <v>7.8250000000000002</v>
+        <v>7.8049999999999997</v>
       </c>
       <c r="D32">
         <f>SUM(D28:D31)</f>
-        <v>4.5350000000000001</v>
+        <v>4.5250000000000004</v>
       </c>
       <c r="F32">
         <f>SUM(F28:F31)</f>
-        <v>7.8250000000000002</v>
+        <v>6.4550000000000001</v>
       </c>
       <c r="G32">
         <f>SUM(G28:G31)</f>
-        <v>4.5350000000000001</v>
+        <v>6.7750000000000004</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1041,23 +1041,23 @@
         <v>16</v>
       </c>
       <c r="C37">
-        <f>0.01*SUM(B2:B5)/4</f>
-        <v>-1.25E-3</v>
+        <f>0.01*((SUM(B2:B5)/4)-(-6.5))</f>
+        <v>6.3750000000000001E-2</v>
       </c>
       <c r="D37">
-        <f>0.01*SUM(C2:C5)/4</f>
-        <v>2.8750000000000001E-2</v>
+        <f>0.01*((SUM(C2:C5)/4)-6)</f>
+        <v>-3.125E-2</v>
       </c>
       <c r="E37">
         <v>1</v>
       </c>
       <c r="F37">
         <f>C37*E37</f>
-        <v>-1.25E-3</v>
+        <v>6.3750000000000001E-2</v>
       </c>
       <c r="G37">
         <f>D37*E37</f>
-        <v>2.8750000000000001E-2</v>
+        <v>-3.125E-2</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1155,19 +1155,19 @@
     <row r="42" spans="1:7">
       <c r="C42">
         <f>SUM(C37:C41)</f>
-        <v>1.7487499999999998</v>
+        <v>1.8137500000000002</v>
       </c>
       <c r="D42">
         <f>SUM(D37:D41)</f>
-        <v>4.7787500000000005</v>
+        <v>4.71875</v>
       </c>
       <c r="F42">
         <f>SUM(F37:F41)</f>
-        <v>0.84874999999999989</v>
+        <v>0.91375000000000028</v>
       </c>
       <c r="G42">
         <f>SUM(G37:G41)</f>
-        <v>4.7787500000000005</v>
+        <v>4.71875</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1176,11 +1176,11 @@
       </c>
       <c r="C45">
         <f>-6.5+C42</f>
-        <v>-4.7512500000000006</v>
+        <v>-4.6862499999999994</v>
       </c>
       <c r="D45">
         <f>6+D42</f>
-        <v>10.77875</v>
+        <v>10.71875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjusted weights to give better behaviour
</commit_message>
<xml_diff>
--- a/etc/calculations.xlsx
+++ b/etc/calculations.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="130405" concurrentCalc="0"/>
+  <calcPr calcId="130404" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>b1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -142,6 +142,10 @@
   </si>
   <si>
     <t>weighted</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Velocity adjustment</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -265,23 +269,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="494715496"/>
-        <c:axId val="494711480"/>
+        <c:axId val="481150280"/>
+        <c:axId val="481234856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="494715496"/>
+        <c:axId val="481150280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="494711480"/>
+        <c:crossAx val="481234856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="494711480"/>
+        <c:axId val="481234856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -289,7 +293,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="494715496"/>
+        <c:crossAx val="481150280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -667,7 +671,7 @@
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -704,7 +708,7 @@
       </c>
       <c r="F2">
         <f t="shared" ref="F2:F8" ca="1" si="0">RANDBETWEEN(0, 5)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -725,7 +729,7 @@
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -746,7 +750,7 @@
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -767,13 +771,13 @@
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -782,7 +786,7 @@
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -799,7 +803,7 @@
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -810,6 +814,9 @@
         <f>SQRT((B2-B3)^2+(C2-C3)^2)</f>
         <v>1.4142135623730951</v>
       </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
@@ -818,6 +825,14 @@
       <c r="B10">
         <f>SQRT((B4-$B$3)^2+(C4-$C$3)^2)</f>
         <v>1.5811388300841898</v>
+      </c>
+      <c r="D10">
+        <f>D8-D3</f>
+        <v>0.33333333333333348</v>
+      </c>
+      <c r="E10">
+        <f>E8-E3</f>
+        <v>-3</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -939,23 +954,23 @@
         <v>17</v>
       </c>
       <c r="C29">
-        <f>D8</f>
-        <v>3.3333333333333335</v>
+        <f>D10</f>
+        <v>0.33333333333333348</v>
       </c>
       <c r="D29">
-        <f>E8</f>
-        <v>2</v>
+        <f>E10</f>
+        <v>-3</v>
       </c>
       <c r="E29">
         <v>1</v>
       </c>
       <c r="F29">
         <f t="shared" ref="F29:F31" si="1">C29*E29</f>
-        <v>3.3333333333333335</v>
+        <v>0.33333333333333348</v>
       </c>
       <c r="G29">
         <f t="shared" ref="G29:G31" si="2">E29*D29</f>
-        <v>2</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1010,19 +1025,19 @@
       </c>
       <c r="C32">
         <f>SUM(C28:C31)</f>
-        <v>7.8049999999999997</v>
+        <v>4.8049999999999997</v>
       </c>
       <c r="D32">
         <f>SUM(D28:D31)</f>
-        <v>4.5250000000000004</v>
+        <v>-0.47499999999999964</v>
       </c>
       <c r="F32">
         <f>SUM(F28:F31)</f>
-        <v>6.4550000000000001</v>
+        <v>3.4550000000000001</v>
       </c>
       <c r="G32">
         <f>SUM(G28:G31)</f>
-        <v>6.7750000000000004</v>
+        <v>1.7749999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1186,7 +1201,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>

<commit_message>
I think I added a goal adjustment
</commit_message>
<xml_diff>
--- a/etc/calculations.xlsx
+++ b/etc/calculations.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="130404" concurrentCalc="0"/>
+  <calcPr calcId="130405" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>b1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -81,10 +81,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>For B2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>center of mass adjustment</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -146,6 +142,22 @@
   </si>
   <si>
     <t>Velocity adjustment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal adjustment for b2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>For B2 and goal -3 5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal-adjustment</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -269,23 +281,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="481150280"/>
-        <c:axId val="481234856"/>
+        <c:axId val="586990360"/>
+        <c:axId val="587082648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="481150280"/>
+        <c:axId val="586990360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="481234856"/>
+        <c:crossAx val="587082648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="481234856"/>
+        <c:axId val="587082648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -293,7 +305,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="481150280"/>
+        <c:crossAx val="586990360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -324,7 +336,7 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>584200</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -668,10 +680,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -708,7 +720,7 @@
       </c>
       <c r="F2">
         <f t="shared" ref="F2:F8" ca="1" si="0">RANDBETWEEN(0, 5)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -729,7 +741,7 @@
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -750,7 +762,7 @@
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -771,13 +783,13 @@
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -786,7 +798,7 @@
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -803,7 +815,7 @@
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -815,7 +827,7 @@
         <v>1.4142135623730951</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -844,10 +856,21 @@
         <v>8.6023252670426267</v>
       </c>
     </row>
+    <row r="12" spans="1:6">
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+    </row>
     <row r="13" spans="1:6">
       <c r="B13" t="s">
         <v>4</v>
       </c>
+      <c r="D13">
+        <v>-3</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
@@ -873,6 +896,19 @@
       <c r="C15">
         <f>C4-C3</f>
         <v>1.5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="D16">
+        <f>D13-B3</f>
+        <v>-5</v>
+      </c>
+      <c r="E16">
+        <f>E13-C3</f>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -905,7 +941,7 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23">
         <v>100</v>
@@ -913,21 +949,21 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="E27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" t="s">
         <v>26</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>27</v>
-      </c>
-      <c r="G27" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C28">
         <f>B22/B23</f>
@@ -938,20 +974,20 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F28">
         <f>C28*E28</f>
-        <v>-2.8333333333333335E-2</v>
+        <v>-0.56666666666666665</v>
       </c>
       <c r="G28">
         <f>E28*D28</f>
-        <v>2.5000000000000001E-2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C29">
         <f>D10</f>
@@ -962,20 +998,20 @@
         <v>-3</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="F29">
         <f t="shared" ref="F29:F31" si="1">C29*E29</f>
-        <v>0.33333333333333348</v>
+        <v>3.3333333333333347E-2</v>
       </c>
       <c r="G29">
-        <f t="shared" ref="G29:G31" si="2">E29*D29</f>
-        <v>-3</v>
+        <f t="shared" ref="G29:G32" si="2">E29*D29</f>
+        <v>-0.30000000000000004</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C30">
         <f>B17</f>
@@ -986,20 +1022,20 @@
         <v>-2.5</v>
       </c>
       <c r="E30">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="F30">
         <f t="shared" si="1"/>
-        <v>0.15000000000000002</v>
+        <v>0.44999999999999996</v>
       </c>
       <c r="G30">
         <f t="shared" si="2"/>
-        <v>-0.25</v>
+        <v>-0.75</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C31">
         <v>3</v>
@@ -1021,124 +1057,125 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C32">
+        <f>-3-B3</f>
+        <v>-5</v>
+      </c>
+      <c r="D32">
+        <v>5</v>
+      </c>
+      <c r="E32">
+        <v>0.2</v>
+      </c>
+      <c r="F32">
+        <f>C32*E32</f>
+        <v>-1</v>
+      </c>
+      <c r="G32">
+        <f>D32*E32</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33">
         <f>SUM(C28:C31)</f>
         <v>4.8049999999999997</v>
       </c>
-      <c r="D32">
+      <c r="D33">
         <f>SUM(D28:D31)</f>
         <v>-0.47499999999999964</v>
       </c>
-      <c r="F32">
-        <f>SUM(F28:F31)</f>
-        <v>3.4550000000000001</v>
-      </c>
-      <c r="G32">
-        <f>SUM(G28:G31)</f>
-        <v>1.7749999999999999</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" t="s">
-        <v>25</v>
-      </c>
-      <c r="E36" t="s">
-        <v>29</v>
-      </c>
-      <c r="F36" t="s">
-        <v>30</v>
+      <c r="F33">
+        <f>SUM(F28:F32)</f>
+        <v>1.9166666666666665</v>
+      </c>
+      <c r="G33">
+        <f>SUM(G28:G32)</f>
+        <v>5.45</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>16</v>
-      </c>
-      <c r="C37">
+        <v>24</v>
+      </c>
+      <c r="E37" t="s">
+        <v>28</v>
+      </c>
+      <c r="F37" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38">
         <f>0.01*((SUM(B2:B5)/4)-(-6.5))</f>
         <v>6.3750000000000001E-2</v>
       </c>
-      <c r="D37">
+      <c r="D38">
         <f>0.01*((SUM(C2:C5)/4)-6)</f>
         <v>-3.125E-2</v>
       </c>
-      <c r="E37">
-        <v>1</v>
-      </c>
-      <c r="F37">
-        <f>C37*E37</f>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <f>C38*E38</f>
         <v>6.3750000000000001E-2</v>
       </c>
-      <c r="G37">
-        <f>D37*E37</f>
+      <c r="G38">
+        <f>D38*E38</f>
         <v>-3.125E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
-      <c r="A38" t="s">
-        <v>17</v>
-      </c>
-      <c r="C38">
+    <row r="39" spans="1:7">
+      <c r="A39" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39">
         <f>SUM(D2:D5)/4</f>
         <v>3.25</v>
       </c>
-      <c r="D38">
+      <c r="D39">
         <f>SUM(E2:E5)/4</f>
         <v>2.75</v>
       </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-      <c r="F38">
-        <f t="shared" ref="F38:F41" si="3">C38*E38</f>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <f t="shared" ref="F39:F43" si="3">C39*E39</f>
         <v>3.25</v>
       </c>
-      <c r="G38">
-        <f t="shared" ref="G38:G41" si="4">D38*E38</f>
+      <c r="G39">
+        <f t="shared" ref="G39:G43" si="4">D39*E39</f>
         <v>2.75</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
-      <c r="A39" t="s">
-        <v>18</v>
-      </c>
-      <c r="C39">
+    <row r="40" spans="1:7">
+      <c r="A40" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40">
         <f>-6.5-B5</f>
         <v>-1.5</v>
       </c>
-      <c r="D39">
+      <c r="D40">
         <f>6-C5</f>
         <v>0</v>
       </c>
-      <c r="E39">
-        <v>1</v>
-      </c>
-      <c r="F39">
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
         <f t="shared" si="3"/>
         <v>-1.5</v>
-      </c>
-      <c r="G39">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" t="s">
-        <v>21</v>
-      </c>
-      <c r="C40">
-        <v>1</v>
-      </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-      <c r="E40">
-        <v>0.1</v>
-      </c>
-      <c r="F40">
-        <f t="shared" si="3"/>
-        <v>0.1</v>
       </c>
       <c r="G40">
         <f t="shared" si="4"/>
@@ -1147,60 +1184,107 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C41">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E41">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="F41">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v>0.1</v>
       </c>
       <c r="G41">
         <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42">
+        <f>-3+6.5</f>
+        <v>3.5</v>
+      </c>
+      <c r="D42">
+        <f>5-6</f>
+        <v>-1</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <f>C42*E42</f>
+        <v>3.5</v>
+      </c>
+      <c r="G42">
+        <f>D42*E42</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43">
+        <v>-1</v>
+      </c>
+      <c r="D43">
         <v>2</v>
       </c>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="C42">
-        <f>SUM(C37:C41)</f>
-        <v>1.8137500000000002</v>
-      </c>
-      <c r="D42">
-        <f>SUM(D37:D41)</f>
-        <v>4.71875</v>
-      </c>
-      <c r="F42">
-        <f>SUM(F37:F41)</f>
-        <v>0.91375000000000028</v>
-      </c>
-      <c r="G42">
-        <f>SUM(G37:G41)</f>
-        <v>4.71875</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45" t="s">
-        <v>23</v>
-      </c>
-      <c r="C45">
-        <f>-6.5+C42</f>
-        <v>-4.6862499999999994</v>
-      </c>
-      <c r="D45">
-        <f>6+D42</f>
-        <v>10.71875</v>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="C44">
+        <f>SUM(C38:C43)</f>
+        <v>5.3137500000000006</v>
+      </c>
+      <c r="D44">
+        <f>SUM(D38:D43)</f>
+        <v>3.71875</v>
+      </c>
+      <c r="F44">
+        <f>SUM(F38:F43)</f>
+        <v>4.4137500000000003</v>
+      </c>
+      <c r="G44">
+        <f>SUM(G38:G43)</f>
+        <v>3.71875</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" t="s">
+        <v>22</v>
+      </c>
+      <c r="C47">
+        <f>-6.5+C44</f>
+        <v>-1.1862499999999994</v>
+      </c>
+      <c r="D47">
+        <f>6+D44</f>
+        <v>9.71875</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>

<commit_message>
added goal weight to total tests
</commit_message>
<xml_diff>
--- a/etc/calculations.xlsx
+++ b/etc/calculations.xlsx
@@ -195,8 +195,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -683,7 +684,7 @@
   <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -741,7 +742,7 @@
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -762,7 +763,7 @@
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -789,7 +790,7 @@
     <row r="6" spans="1:6">
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -798,7 +799,7 @@
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1139,23 +1140,23 @@
         <v>16</v>
       </c>
       <c r="C39">
-        <f>SUM(D2:D5)/4</f>
-        <v>3.25</v>
+        <f>SUM(D2:D5)/4-(-1)</f>
+        <v>4.25</v>
       </c>
       <c r="D39">
-        <f>SUM(E2:E5)/4</f>
-        <v>2.75</v>
+        <f>SUM(E2:E5)/4-2</f>
+        <v>0.75</v>
       </c>
       <c r="E39">
         <v>1</v>
       </c>
       <c r="F39">
         <f t="shared" ref="F39:F43" si="3">C39*E39</f>
-        <v>3.25</v>
+        <v>4.25</v>
       </c>
       <c r="G39">
         <f t="shared" ref="G39:G43" si="4">D39*E39</f>
-        <v>2.75</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1212,7 +1213,7 @@
         <f>-3+6.5</f>
         <v>3.5</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="1">
         <f>5-6</f>
         <v>-1</v>
       </c>
@@ -1253,19 +1254,19 @@
     <row r="44" spans="1:7">
       <c r="C44">
         <f>SUM(C38:C43)</f>
-        <v>5.3137500000000006</v>
+        <v>6.3137499999999998</v>
       </c>
       <c r="D44">
         <f>SUM(D38:D43)</f>
-        <v>3.71875</v>
+        <v>1.71875</v>
       </c>
       <c r="F44">
         <f>SUM(F38:F43)</f>
-        <v>4.4137500000000003</v>
+        <v>5.4137500000000003</v>
       </c>
       <c r="G44">
         <f>SUM(G38:G43)</f>
-        <v>3.71875</v>
+        <v>1.71875</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -1274,11 +1275,11 @@
       </c>
       <c r="C47">
         <f>-6.5+C44</f>
-        <v>-1.1862499999999994</v>
+        <v>-0.18625000000000025</v>
       </c>
       <c r="D47">
         <f>6+D44</f>
-        <v>9.71875</v>
+        <v>7.71875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed more tests for the goal adjustment
</commit_message>
<xml_diff>
--- a/etc/calculations.xlsx
+++ b/etc/calculations.xlsx
@@ -684,7 +684,7 @@
   <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -721,7 +721,7 @@
       </c>
       <c r="F2">
         <f t="shared" ref="F2:F8" ca="1" si="0">RANDBETWEEN(0, 5)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -742,7 +742,7 @@
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -763,7 +763,7 @@
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -790,7 +790,7 @@
     <row r="6" spans="1:6">
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -816,7 +816,7 @@
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1065,7 +1065,8 @@
         <v>-5</v>
       </c>
       <c r="D32">
-        <v>5</v>
+        <f>5-C3</f>
+        <v>4</v>
       </c>
       <c r="E32">
         <v>0.2</v>
@@ -1076,7 +1077,7 @@
       </c>
       <c r="G32">
         <f>D32*E32</f>
-        <v>1</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1084,12 +1085,12 @@
         <v>18</v>
       </c>
       <c r="C33">
-        <f>SUM(C28:C31)</f>
-        <v>4.8049999999999997</v>
+        <f>SUM(C28:C32)</f>
+        <v>-0.19500000000000028</v>
       </c>
       <c r="D33">
-        <f>SUM(D28:D31)</f>
-        <v>-0.47499999999999964</v>
+        <f>SUM(D28:D32)</f>
+        <v>3.5250000000000004</v>
       </c>
       <c r="F33">
         <f>SUM(F28:F32)</f>
@@ -1097,7 +1098,7 @@
       </c>
       <c r="G33">
         <f>SUM(G28:G32)</f>
-        <v>5.45</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1194,11 +1195,11 @@
         <v>0</v>
       </c>
       <c r="E41">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="F41">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="G41">
         <f t="shared" si="4"/>
@@ -1262,7 +1263,7 @@
       </c>
       <c r="F44">
         <f>SUM(F38:F43)</f>
-        <v>5.4137500000000003</v>
+        <v>6.3137499999999998</v>
       </c>
       <c r="G44">
         <f>SUM(G38:G43)</f>
@@ -1281,8 +1282,17 @@
         <f>6+D44</f>
         <v>7.71875</v>
       </c>
+      <c r="F47">
+        <f>-6.5+F44</f>
+        <v>-0.18625000000000025</v>
+      </c>
+      <c r="G47">
+        <f>-6+G44</f>
+        <v>-4.28125</v>
+      </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>